<commit_message>
Changed FSM for primary schools to be percentage of P6 and P7 pupils, so excluding universal provision. Also changed guidance text.
</commit_message>
<xml_diff>
--- a/app/modules/text_content/FAQ.xlsx
+++ b/app/modules/text_content/FAQ.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SEED\Spreadsheets\ScotXed\Insight\Analysis\NIFIER and SID\School Information Dashboard\SID RAP\School Information Dashboards\app\modules\text_content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SEED\Spreadsheets\ScotXed\Insight\Analysis\NIFIER and SID\School Information Dashboard\SID RAP\school-information-dashboard\app\modules\text_content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3ED67FF-1F59-48E6-8A3F-311AE21F98D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE27370-FA70-401E-84B9-3A9996D94389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FAQ" sheetId="1" r:id="rId1"/>
@@ -283,6 +283,111 @@
     <t xml:space="preserve">This information is included as it provides useful context for children and young people’s achievement and attainment.  </t>
   </si>
   <si>
+    <t>The Scottish Credit and Qualifications Framework is Scotland's national qualifications framework.  The SCQF supports lifelong learning and can:  help people of all ages and circumstances to access appropriate education and training over their lifetime; and help employers, learners and the general public to understand the full range of Scottish qualifications, how they relate to each other and to other forms of learning, and how different types of qualification can contribute to improving the skills of the workforce.
+The SCQF has 12 levels which indicate the level of difficulty of a qualification.  SCQF levels allow broad comparisons to be made between qualifications and learning. 
+Examples of some of the SCQF level qualifications are: SCQF Level 3 – SQA National 3, SCQF Level 5 – SQA National 5, SQA Modern Apprenticeship and SQA Scottish Vocational Qualification (SVQ) 2, SCQF Level 7 – SQA Advanced Higher, SQA Higher National Certificate (HNC) and SQA Scottish Baccalaureates.
+More information can be found on the SCQF website and the SQA website. Links to these can be found in the ‘Useful Links’ section below.</t>
+  </si>
+  <si>
+    <t>The secondary school dashboard uses some information from the “Insight” tool.  Insight captures information on attainment and qualifications that school leavers from S4, S5 and S6 have achieved.  Insight also provides information on school leaver destinations – i.e. whether school pupils go onto college, university, or employment. 
+Insight is a professional tool, aimed at teachers and other staff, used to help secondary schools and local authorities identify areas of success and where improvements can be made.  Its key focus is on detailed information about the attainment and destinations of school leavers.  Much of the attainment information is based on latest and best awards in each subject.  This means that, for example, if someone has a National 5 and a Higher in Mathematics, it is the Higher award which is counted.
+Insight does not include data relating to attainment in S1-S3.
+Although Insight provides data on the attainment of a wide range of Scottish Credit and Qualifications Framework (SCQF) awards from a range of providers, not all SCQF achievement awards are included.
+More information on ‘Insight’ is available on the Scottish Government website. A link to this website can be found in the ‘Useful Links’ section below.</t>
+  </si>
+  <si>
+    <t>The 'virtual comparator' is a sample group of pupils from other parts of Scotland who have the same characteristics as the young people in your school.   A ‘virtual comparator’ allows the results of a school to be put into context based on the characteristics of its school leavers.
+For each school leaver, ten matching school leavers are randomly selected based on gender, additional support needs, stage of leaving school (S4, S5 or S6) and the social context in which they live (Scottish Index of Multiple Deprivation).  These characteristics were selected due to their significance in explaining differences in the attainment and destinations of school leavers in Scotland.</t>
+  </si>
+  <si>
+    <t>The tariff score for a learner is the total number of tariff points for the awards they achieve, taking account of only their latest and best attainment in each subject.  This means that, for example, if someone has a National 5 and a Higher in Mathematics, it is the points for the Higher award which are counted.
+Subject courses and individual units are awarded tariff points.  The number of tariff points awarded depends on:  the SCQF level of the course or unit; whether the full course has been undertaken and assessed; and the grade achieved for the course. 
+The average tariff scores of a school's leavers are not directly comparable with other schools'.  This is because they are influenced by a range of factors including the number of subjects young people take in the senior phase.
+The tariff score used on Insight should not be confused with the term 'tariff' as used by the Universities and Colleges Admissions Service (UCAS), which is calculated differently.</t>
+  </si>
+  <si>
+    <t>A young person of school leaving age who left secondary school (from S4, S5 or S6) during or at the end of the school year.
+School leavers are recorded against the school at which they were present in the pupil census in September. Young people who move to another school or outwith Scotland are not included.</t>
+  </si>
+  <si>
+    <t>Information is collected by Skills Development Scotland on what young people do when they leave school.  This information is referred to as “school leaver destinations”.
+Scottish education aims to support all young people to have a 'positive destination' when they leave school.  Positive destinations include: higher education, further education, training, voluntary work, employment, activity agreements.
+Details about a leaver's destination are only included in the measure if a link can be made between the leaver's Skills Development Scotland destination record and a Pupil Census record with stage S4, S5 or S6 for the same academic year.  In addition, the young person must not have a Pupil Census record in the following academic year in a senior phase stage (S4-S6).</t>
+  </si>
+  <si>
+    <t>The percentage of Secondary 3 (S3) pupils achieving the Curriculum for Excellence (CfE) level relevant to their stage (i.e. CfE 3rd Level or better) is included on the secondary school dashboard.  However, the secondary school dashboard does not include the comparator chart showing how S3 pupils in a school compare, on average, to similar pupils across Scotland.  This is because comparator information, based on senior phase school leaver qualifications and destinations, has been included on the  secondary schools dashboard. This information has been available for a number of years and shows you how a secondary school is performing against their virtual comparator.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of pupils is the number of pupils who are based on the roll of a school in the area/school selected (Note:  each pupil can only be based on one school roll even if they attend more than one school to receive their education). </t>
+  </si>
+  <si>
+    <t>The dashboard does not show the number of teachers who are physically present in the school.  Instead, teacher numbers are calculated in terms of those working full time hours.  Full-Time Equivalents (FTE).  For example, in a school where there are 10 actual teachers, 9 of whom work full time, and 1 of whom works 2 days a week, the dashboard will show 9.4 teachers working at the school.  This will be shown as 9.4 FTEs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The pupil/teacher ratio shows the number of pupils for each full-time equivalent teacher.  For example, if an area/school has 120 pupils and has 9.5 FTE teachers, then the pupil/teacher ratio would be 12.6 (i.e. 12.6 pupils per 1 FTE teacher). </t>
+  </si>
+  <si>
+    <t>A class is a group of pupils normally supervised by one teacher.  However, when a class is large and cannot be split, for instance an additional classroom is not available, team teaching may be used.  Team teaching is when two teachers are present in the class at all times.  When this occurs, the pupil teacher ratio will not exceed maximum class size regulations.   
+All class size calculations treat a two-teacher class as two classes with half the pupils in each.  Total average class size is calculated by dividing the number of pupils by the number of classes.  Average class size for pupils in a particular stage (or range of stages) uses the average class size experienced by pupils, which therefore takes into account the number of pupils experiencing each class size.  For example, if three pupils are in a class of three and one pupil is in a class of one, the average of three, three, three and one is 2.5.
+Maximum class sizes in primary schools are as follows:
+25 for pupils in P1
+30 for single stage class P2 or P3
+33 for single stage class P4-P7
+25 for composite stage class (a composite class is a class of pupils from two or more stages)</t>
+  </si>
+  <si>
+    <t>The Scottish Index of Multiple Deprivation identifies small area concentrations of multiple deprivation across all of Scotland in a consistent way.  It allows policies and funding to be put in place to tackle issues associated with multiple deprivation.
+Scotland has been split up into small geographical areas called datazones.  They have an average population of between 500 and 1,000 residents and contain households with similar social characteristics.  They sit within local authority boundaries and, where possible, respect physical boundaries and natural communities.
+A number of factors are taken into consideration when calculating how deprived a particular geographical area or ‘datazones’ is. (employment, health, access to services, for example) Once analysed, all datazones are then ordered and can be divided into deciles (10ths) or quintiles (5ths).  
+More information on the Scottish Index of Multiple Deprivation can be found on the SIMD website. A link to this is available in the ‘Useful Links’ section below</t>
+  </si>
+  <si>
+    <t>9.2 What are Additional Support Needs?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Education (Additional Support for Learning) Scotland Act 2004 (as amended) states that a child or young person has an additional support need where they need additional support in order to overcome barriers and benefit from school education.  The Act also states that education authorities must have arrangements in place to identify pupils with Additional Support Needs (ASN) and from among them, those who may require a Co-ordinated Support Plan (CSP) or Individualised Educational Programme (IEP).  Education authorities must also be able to identify the reason(s) that additional support is needed.  Child plans are single or multi agency plans based on an assessment guided by the Getting it Right for every Child National Practice Model. 
+ASN figures also includes 'other' types of support.  'Other' type refers to additional support needs which have been identified and are being supported but which do not fall within the subcategories of need collected in the pupil census.  These may be needs which are of short-term duration, or which do not need significant differentiation of learning and teaching to overcome barriers to learning. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pupils make progress in acquiring English as an Additional Language (EAL) in different ways and at different rates.  Four broad stages in this development are included in the “EAL” category: New to English, Early Acquisition, Developing competence, and Competent 
+All other categories recorded as counted as “No EAL”, these being: Fluent, English as a “first-language”, Complex learning difficulties affecting communication make assessment for level of English as an Additional Language inappropriate, and Not assessed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parents/guardians are asked to declare the ethnic background of their child or young person - up to and including stage S2.  Pupils in stage S3 or above may declare their own ethnic background.  The purpose of this is to record the ethnic background of individuals, not their nationality.  For example, those of Asian background are asked to select one of the categories Indian, Pakistani, Bangladeshi, Chinese, or other Asian background, irrespective of whether they were born in Scotland or any other part of the UK.  ‘White Other’ is to be used for all non-UK White backgrounds, including Republic of Ireland.  The ‘Not Known’ category shown here includes individual who did not wish their ethnic background to be recorded (i.e. ‘Not Disclosed’) as well as where no response was made by the appropriate individual (i.e. ‘Not Known’).   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The 'Taught in Gaelic' category includes pupils based in primary classes whose aim is be to bring pupils to fluency in the language and to teach a range of subjects through the medium of Gaelic.  In secondary, this will include pupils who are being taught subjects other than Gaelic language (often referred to as Gàidhlig) through the  medium of Gaelic. 
+It also includes secondary pupils (who have gone through Gaelic Medium Education at primary school and are therefore fluent in Gaelic) who are in Gàidhlig classes.  It also include pupils who are learning Gaelic (but not as a fluent speaker), and are learning this through the medium of English and Gaelic.  These classes will operate in a similar way to any other language being learned such as French or German at both primary or secondary school. </t>
+  </si>
+  <si>
+    <t>The Scottish Government Urban Rural Classification provides a standard definition of rural areas in Scotland. This classification is updated every two years to incorporate the most recent Small Area Population Estimates (SAPE) produced by National Records of Scotland (NRS) and Royal Mail Postcode Address File (PAF).
+The data on this dashboard is a combination of 6 fold Urban Rural Classification data. 
+Pupils who live in Large Urban Areas (settlements of 125,000 or more people) or Other Urban Areas (settlements of 10,000 to 124,999 people) are recorded as living in Urban Areas.
+Pupils who live in Accessible Small Towns (settlements of 3,000 to 9,999 people and within 30 minutes drive of a settlement of 10,000 or more) or Remote Small Towns (settlements of 3,000 to 9,999 people and with a drive time of over 30 minutes to a settlement of 10,000 or more) are recorded as living in Small Towns.
+Pupils who live in Accessible Rural (areas with a population of less than 3,000 people and within a 30 minute drive of a settlement of 10,000 or more) or Remote Rural (areas with a population of less than 3,000 people and with a drive time of over 30 minutes to a settlement of 10,000 or more) are recorded as living in Rural Areas.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The School Information Dashboard is part of the Government’s mission to support excellence and equity in Scottish education.  The primary purpose is to drive improvement for children and young people.
+The Scottish Government is committed to ensuring that the achievement of schools is made more coherent and transparent. This is why we’ve updated the way we display the data you can find through Parentzone Scotland, or directly from the Scottish Government’s website.  The School Information Dashboard brings together a range of information - some of which has been available in the past through Parentzone Scotland or the Scottish Government website - along with some new elements. </t>
+  </si>
+  <si>
+    <t>If you have a technical question about how the data has been gathered, or about this website, you should email school.stats@gov.scot.
+If you have any questions about what the information means to you, or your child/young person, or  you wish to understand what this means in relation to a particular school, you should contact the school directly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The dashboard shows the most up-to-date information that is available.   However, it is important to remember that some of this information may be up to two years old.  This is because some of the data is only collected by the Scottish Government on a two-yearly basis. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The data that is shown on the dashboard is collected at different times throughout the year.  The dashboard is updated in December and April each year.  </t>
+  </si>
+  <si>
+    <t>If you have a technical question about how the data has been gathered, or about this website, you should email school.stats@gov.scot.
+If you have any questions about what the information means to you, or your child or young person, or you wish to understand more about what it means in relation to a particular school, you should contact the school directly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The national criteria for eligibility to free school meals include all those pupils within families who receive Income Support, Income-based Job Seekers Allowance or any income related element of Employment and Support Allowance.  Pupils within families who receive support under Part VI of the Immigration and Asylum Act 1999 were also entitled.  Pupils whose parents or carers receive Child Tax Credit, do not receive Working Tax Credit and had an annual income (as assessed by the Inland Revenue) of below £16,105 (from April 2013) were also entitled.  Pupils whose parents or carers are in receipt of both maximum Child Tax Credit and maximum Working Tax Credit and their income is under £6,420 were also entitled (from August 2009).  Pupils whose parents or carers are in receipt of Universal Credit and their monthly earned income does not exceed £610 were also entitled (from August 2017).  Pupils in school education who receive any of these benefits in their own right are also entitled to receive free school meals.  In addition, eligibility for free school meals was extended to all pupils in P1-P3 in January 2015, to all pupils in P4 in August 2021 and then to all pupils in P5 in January 2022. </t>
+  </si>
+  <si>
     <t>The 9 characteristics used are:
 Whether a pupil is male or female
 The SIMD Decile a pupil lives in, based on their postcode ( SIMD Decile 1 = most deprived, SIMD Decile 10 = least deprived)
@@ -293,114 +398,9 @@
 Whether a pupil has ethnicity recorded as 'White UK', 'White Other', 'Ethnic Minority' or 'Not known/disclosed'
 Whether a pupil speaks English as an Additional Language or not
 Whether a pupil is working towards individual milestones or not**
-*This is not used when looking at P1 pupils since all pupils in P1 are registered for free school meals.
+*This is not used when looking at P1-P5 pupils since all pupils in P1-P5 are registered for free school meals.
 **This is based on the Achievement of a Curriculum for Excellence level return. For calculation purposes, pupils working towards their own individual milestones are classified as 'not yet achieving CfE Early Level'.
 (see question 4.5)</t>
-  </si>
-  <si>
-    <t>The Scottish Credit and Qualifications Framework is Scotland's national qualifications framework.  The SCQF supports lifelong learning and can:  help people of all ages and circumstances to access appropriate education and training over their lifetime; and help employers, learners and the general public to understand the full range of Scottish qualifications, how they relate to each other and to other forms of learning, and how different types of qualification can contribute to improving the skills of the workforce.
-The SCQF has 12 levels which indicate the level of difficulty of a qualification.  SCQF levels allow broad comparisons to be made between qualifications and learning. 
-Examples of some of the SCQF level qualifications are: SCQF Level 3 – SQA National 3, SCQF Level 5 – SQA National 5, SQA Modern Apprenticeship and SQA Scottish Vocational Qualification (SVQ) 2, SCQF Level 7 – SQA Advanced Higher, SQA Higher National Certificate (HNC) and SQA Scottish Baccalaureates.
-More information can be found on the SCQF website and the SQA website. Links to these can be found in the ‘Useful Links’ section below.</t>
-  </si>
-  <si>
-    <t>The secondary school dashboard uses some information from the “Insight” tool.  Insight captures information on attainment and qualifications that school leavers from S4, S5 and S6 have achieved.  Insight also provides information on school leaver destinations – i.e. whether school pupils go onto college, university, or employment. 
-Insight is a professional tool, aimed at teachers and other staff, used to help secondary schools and local authorities identify areas of success and where improvements can be made.  Its key focus is on detailed information about the attainment and destinations of school leavers.  Much of the attainment information is based on latest and best awards in each subject.  This means that, for example, if someone has a National 5 and a Higher in Mathematics, it is the Higher award which is counted.
-Insight does not include data relating to attainment in S1-S3.
-Although Insight provides data on the attainment of a wide range of Scottish Credit and Qualifications Framework (SCQF) awards from a range of providers, not all SCQF achievement awards are included.
-More information on ‘Insight’ is available on the Scottish Government website. A link to this website can be found in the ‘Useful Links’ section below.</t>
-  </si>
-  <si>
-    <t>The 'virtual comparator' is a sample group of pupils from other parts of Scotland who have the same characteristics as the young people in your school.   A ‘virtual comparator’ allows the results of a school to be put into context based on the characteristics of its school leavers.
-For each school leaver, ten matching school leavers are randomly selected based on gender, additional support needs, stage of leaving school (S4, S5 or S6) and the social context in which they live (Scottish Index of Multiple Deprivation).  These characteristics were selected due to their significance in explaining differences in the attainment and destinations of school leavers in Scotland.</t>
-  </si>
-  <si>
-    <t>The tariff score for a learner is the total number of tariff points for the awards they achieve, taking account of only their latest and best attainment in each subject.  This means that, for example, if someone has a National 5 and a Higher in Mathematics, it is the points for the Higher award which are counted.
-Subject courses and individual units are awarded tariff points.  The number of tariff points awarded depends on:  the SCQF level of the course or unit; whether the full course has been undertaken and assessed; and the grade achieved for the course. 
-The average tariff scores of a school's leavers are not directly comparable with other schools'.  This is because they are influenced by a range of factors including the number of subjects young people take in the senior phase.
-The tariff score used on Insight should not be confused with the term 'tariff' as used by the Universities and Colleges Admissions Service (UCAS), which is calculated differently.</t>
-  </si>
-  <si>
-    <t>A young person of school leaving age who left secondary school (from S4, S5 or S6) during or at the end of the school year.
-School leavers are recorded against the school at which they were present in the pupil census in September. Young people who move to another school or outwith Scotland are not included.</t>
-  </si>
-  <si>
-    <t>Information is collected by Skills Development Scotland on what young people do when they leave school.  This information is referred to as “school leaver destinations”.
-Scottish education aims to support all young people to have a 'positive destination' when they leave school.  Positive destinations include: higher education, further education, training, voluntary work, employment, activity agreements.
-Details about a leaver's destination are only included in the measure if a link can be made between the leaver's Skills Development Scotland destination record and a Pupil Census record with stage S4, S5 or S6 for the same academic year.  In addition, the young person must not have a Pupil Census record in the following academic year in a senior phase stage (S4-S6).</t>
-  </si>
-  <si>
-    <t>The percentage of Secondary 3 (S3) pupils achieving the Curriculum for Excellence (CfE) level relevant to their stage (i.e. CfE 3rd Level or better) is included on the secondary school dashboard.  However, the secondary school dashboard does not include the comparator chart showing how S3 pupils in a school compare, on average, to similar pupils across Scotland.  This is because comparator information, based on senior phase school leaver qualifications and destinations, has been included on the  secondary schools dashboard. This information has been available for a number of years and shows you how a secondary school is performing against their virtual comparator.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of pupils is the number of pupils who are based on the roll of a school in the area/school selected (Note:  each pupil can only be based on one school roll even if they attend more than one school to receive their education). </t>
-  </si>
-  <si>
-    <t>The dashboard does not show the number of teachers who are physically present in the school.  Instead, teacher numbers are calculated in terms of those working full time hours.  Full-Time Equivalents (FTE).  For example, in a school where there are 10 actual teachers, 9 of whom work full time, and 1 of whom works 2 days a week, the dashboard will show 9.4 teachers working at the school.  This will be shown as 9.4 FTEs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The pupil/teacher ratio shows the number of pupils for each full-time equivalent teacher.  For example, if an area/school has 120 pupils and has 9.5 FTE teachers, then the pupil/teacher ratio would be 12.6 (i.e. 12.6 pupils per 1 FTE teacher). </t>
-  </si>
-  <si>
-    <t>A class is a group of pupils normally supervised by one teacher.  However, when a class is large and cannot be split, for instance an additional classroom is not available, team teaching may be used.  Team teaching is when two teachers are present in the class at all times.  When this occurs, the pupil teacher ratio will not exceed maximum class size regulations.   
-All class size calculations treat a two-teacher class as two classes with half the pupils in each.  Total average class size is calculated by dividing the number of pupils by the number of classes.  Average class size for pupils in a particular stage (or range of stages) uses the average class size experienced by pupils, which therefore takes into account the number of pupils experiencing each class size.  For example, if three pupils are in a class of three and one pupil is in a class of one, the average of three, three, three and one is 2.5.
-Maximum class sizes in primary schools are as follows:
-25 for pupils in P1
-30 for single stage class P2 or P3
-33 for single stage class P4-P7
-25 for composite stage class (a composite class is a class of pupils from two or more stages)</t>
-  </si>
-  <si>
-    <t>The Scottish Index of Multiple Deprivation identifies small area concentrations of multiple deprivation across all of Scotland in a consistent way.  It allows policies and funding to be put in place to tackle issues associated with multiple deprivation.
-Scotland has been split up into small geographical areas called datazones.  They have an average population of between 500 and 1,000 residents and contain households with similar social characteristics.  They sit within local authority boundaries and, where possible, respect physical boundaries and natural communities.
-A number of factors are taken into consideration when calculating how deprived a particular geographical area or ‘datazones’ is. (employment, health, access to services, for example) Once analysed, all datazones are then ordered and can be divided into deciles (10ths) or quintiles (5ths).  
-More information on the Scottish Index of Multiple Deprivation can be found on the SIMD website. A link to this is available in the ‘Useful Links’ section below</t>
-  </si>
-  <si>
-    <t>9.2 What are Additional Support Needs?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Education (Additional Support for Learning) Scotland Act 2004 (as amended) states that a child or young person has an additional support need where they need additional support in order to overcome barriers and benefit from school education.  The Act also states that education authorities must have arrangements in place to identify pupils with Additional Support Needs (ASN) and from among them, those who may require a Co-ordinated Support Plan (CSP) or Individualised Educational Programme (IEP).  Education authorities must also be able to identify the reason(s) that additional support is needed.  Child plans are single or multi agency plans based on an assessment guided by the Getting it Right for every Child National Practice Model. 
-ASN figures also includes 'other' types of support.  'Other' type refers to additional support needs which have been identified and are being supported but which do not fall within the subcategories of need collected in the pupil census.  These may be needs which are of short-term duration, or which do not need significant differentiation of learning and teaching to overcome barriers to learning. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pupils make progress in acquiring English as an Additional Language (EAL) in different ways and at different rates.  Four broad stages in this development are included in the “EAL” category: New to English, Early Acquisition, Developing competence, and Competent 
-All other categories recorded as counted as “No EAL”, these being: Fluent, English as a “first-language”, Complex learning difficulties affecting communication make assessment for level of English as an Additional Language inappropriate, and Not assessed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parents/guardians are asked to declare the ethnic background of their child or young person - up to and including stage S2.  Pupils in stage S3 or above may declare their own ethnic background.  The purpose of this is to record the ethnic background of individuals, not their nationality.  For example, those of Asian background are asked to select one of the categories Indian, Pakistani, Bangladeshi, Chinese, or other Asian background, irrespective of whether they were born in Scotland or any other part of the UK.  ‘White Other’ is to be used for all non-UK White backgrounds, including Republic of Ireland.  The ‘Not Known’ category shown here includes individual who did not wish their ethnic background to be recorded (i.e. ‘Not Disclosed’) as well as where no response was made by the appropriate individual (i.e. ‘Not Known’).   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The 'Taught in Gaelic' category includes pupils based in primary classes whose aim is be to bring pupils to fluency in the language and to teach a range of subjects through the medium of Gaelic.  In secondary, this will include pupils who are being taught subjects other than Gaelic language (often referred to as Gàidhlig) through the  medium of Gaelic. 
-It also includes secondary pupils (who have gone through Gaelic Medium Education at primary school and are therefore fluent in Gaelic) who are in Gàidhlig classes.  It also include pupils who are learning Gaelic (but not as a fluent speaker), and are learning this through the medium of English and Gaelic.  These classes will operate in a similar way to any other language being learned such as French or German at both primary or secondary school. </t>
-  </si>
-  <si>
-    <t>The Scottish Government Urban Rural Classification provides a standard definition of rural areas in Scotland. This classification is updated every two years to incorporate the most recent Small Area Population Estimates (SAPE) produced by National Records of Scotland (NRS) and Royal Mail Postcode Address File (PAF).
-The data on this dashboard is a combination of 6 fold Urban Rural Classification data. 
-Pupils who live in Large Urban Areas (settlements of 125,000 or more people) or Other Urban Areas (settlements of 10,000 to 124,999 people) are recorded as living in Urban Areas.
-Pupils who live in Accessible Small Towns (settlements of 3,000 to 9,999 people and within 30 minutes drive of a settlement of 10,000 or more) or Remote Small Towns (settlements of 3,000 to 9,999 people and with a drive time of over 30 minutes to a settlement of 10,000 or more) are recorded as living in Small Towns.
-Pupils who live in Accessible Rural (areas with a population of less than 3,000 people and within a 30 minute drive of a settlement of 10,000 or more) or Remote Rural (areas with a population of less than 3,000 people and with a drive time of over 30 minutes to a settlement of 10,000 or more) are recorded as living in Rural Areas.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The School Information Dashboard is part of the Government’s mission to support excellence and equity in Scottish education.  The primary purpose is to drive improvement for children and young people.
-The Scottish Government is committed to ensuring that the achievement of schools is made more coherent and transparent. This is why we’ve updated the way we display the data you can find through Parentzone Scotland, or directly from the Scottish Government’s website.  The School Information Dashboard brings together a range of information - some of which has been available in the past through Parentzone Scotland or the Scottish Government website - along with some new elements. </t>
-  </si>
-  <si>
-    <t>If you have a technical question about how the data has been gathered, or about this website, you should email school.stats@gov.scot.
-If you have any questions about what the information means to you, or your child/young person, or  you wish to understand what this means in relation to a particular school, you should contact the school directly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The dashboard shows the most up-to-date information that is available.   However, it is important to remember that some of this information may be up to two years old.  This is because some of the data is only collected by the Scottish Government on a two-yearly basis. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">The data that is shown on the dashboard is collected at different times throughout the year.  The dashboard is updated in December and April each year.  </t>
-  </si>
-  <si>
-    <t>If you have a technical question about how the data has been gathered, or about this website, you should email school.stats@gov.scot.
-If you have any questions about what the information means to you, or your child or young person, or you wish to understand more about what it means in relation to a particular school, you should contact the school directly.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The national criteria for eligibility to free school meals include all those pupils within families who receive Income Support, Income-based Job Seekers Allowance or any income related element of Employment and Support Allowance.  Pupils within families who receive support under Part VI of the Immigration and Asylum Act 1999 were also entitled.  Pupils whose parents or carers receive Child Tax Credit, do not receive Working Tax Credit and had an annual income (as assessed by the Inland Revenue) of below £16,105 (from April 2013) were also entitled.  Pupils whose parents or carers are in receipt of both maximum Child Tax Credit and maximum Working Tax Credit and their income is under £6,420 were also entitled (from August 2009).  Pupils whose parents or carers are in receipt of Universal Credit and their monthly earned income does not exceed £610 were also entitled (from August 2017).  Pupils in school education who receive any of these benefits in their own right are also entitled to receive free school meals.  In addition, eligibility for free school meals was extended to all pupils in P1-P3 in January 2015, to all pupils in P4 in August 2021 and then to all pupils in P5 in January 2022. </t>
   </si>
 </sst>
 </file>
@@ -1215,19 +1215,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="B26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="55" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38" style="2" customWidth="1"/>
-    <col min="3" max="3" width="140.28515625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.85546875" style="2"/>
+    <col min="3" max="3" width="140.26953125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="8.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1246,10 +1246,10 @@
         <v>12</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -1304,7 +1304,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -1326,7 +1326,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>3</v>
       </c>
@@ -1334,10 +1334,10 @@
         <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
@@ -1345,10 +1345,10 @@
         <v>21</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
@@ -1356,10 +1356,10 @@
         <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>3</v>
       </c>
@@ -1381,7 +1381,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
@@ -1392,7 +1392,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
@@ -1403,7 +1403,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
@@ -1411,10 +1411,10 @@
         <v>27</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
@@ -1436,7 +1436,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="116" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>5</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>5</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>5</v>
       </c>
@@ -1480,7 +1480,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>5</v>
       </c>
@@ -1491,7 +1491,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="145" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>5</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="174" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>5</v>
       </c>
@@ -1513,7 +1513,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>6</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>6</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
@@ -1543,10 +1543,10 @@
         <v>39</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
@@ -1554,10 +1554,10 @@
         <v>40</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="217.5" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
@@ -1565,10 +1565,10 @@
         <v>41</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1576,10 +1576,10 @@
         <v>42</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="159.5" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>8</v>
       </c>
@@ -1587,10 +1587,10 @@
         <v>43</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="58" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>8</v>
       </c>
@@ -1598,10 +1598,10 @@
         <v>44</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>8</v>
       </c>
@@ -1609,10 +1609,10 @@
         <v>45</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
@@ -1620,10 +1620,10 @@
         <v>46</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>9</v>
       </c>
@@ -1631,10 +1631,10 @@
         <v>47</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>9</v>
       </c>
@@ -1642,10 +1642,10 @@
         <v>48</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>9</v>
       </c>
@@ -1653,10 +1653,10 @@
         <v>49</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="261" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>9</v>
       </c>
@@ -1664,10 +1664,10 @@
         <v>50</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="145" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>10</v>
       </c>
@@ -1675,21 +1675,21 @@
         <v>51</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="130.5" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="149.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:3" ht="149.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>10</v>
       </c>
@@ -1697,10 +1697,10 @@
         <v>52</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>10</v>
       </c>
@@ -1708,10 +1708,10 @@
         <v>53</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="87" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>10</v>
       </c>
@@ -1719,10 +1719,10 @@
         <v>54</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>10</v>
       </c>
@@ -1730,10 +1730,10 @@
         <v>55</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="203" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>10</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>56</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>